<commit_message>
addign articles and excel
</commit_message>
<xml_diff>
--- a/BlountPollutionwithcharts.xlsx
+++ b/BlountPollutionwithcharts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tylerjacobson/Documents/Berkeley/Senior Research Project/Coal Power Plants/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tylerjacobson/Documents/Berkeley/Senior Research Project/Coal Plants/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E51B67FD-5E36-6A41-9509-5F7473338F16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A30B58B-B5C3-0242-BC1E-207E37902A63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="1960" windowWidth="26840" windowHeight="15540" activeTab="2" xr2:uid="{1D80E892-4AC7-4B40-B2CF-48E4B4EABFE8}"/>
   </bookViews>
@@ -17,11 +17,7 @@
     <sheet name="2014 and 2016" sheetId="3" r:id="rId2"/>
     <sheet name="Charts" sheetId="4" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'1998-2012'!$W$3:$W$13</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">'1998-2012'!$W$3:$W$13</definedName>
-  </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>